<commit_message>
Semana 6, Clase 12
</commit_message>
<xml_diff>
--- a/content/week6/AC11y12_optimizacion.xlsx
+++ b/content/week6/AC11y12_optimizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nasalazar/Documents/GitHub/ua-imec2001-hc-202310-s2/content/week6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8912CB11-07DD-324B-A05F-46E8B43045F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE64E6FA-F861-BE44-B898-DBEE113C278C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,14 +17,14 @@
     <sheet name="Práctica No Lineal" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Práctica Lineal'!$A$1</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'Práctica No Lineal'!$A$1</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Práctica Lineal'!$E$2:$E$3</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Práctica No Lineal'!$E$2:$E$3</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Práctica Lineal'!$C$10</definedName>
@@ -40,7 +40,7 @@
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Práctica Lineal'!$C$9</definedName>
     <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Práctica No Lineal'!$C$9</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -50,13 +50,13 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Práctica Lineal'!$A$1</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'Práctica No Lineal'!$A$1</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">6</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Práctica Lineal'!$E$6</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Práctica No Lineal'!$E$6</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
@@ -100,7 +100,7 @@
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
@@ -622,13 +622,17 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="3" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="10" t="s">
@@ -644,7 +648,10 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9">
+        <f>3*E2+4*E3</f>
+        <v>27.5</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
@@ -657,11 +664,16 @@
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <f>2*E2+5*E3</f>
+        <v>30</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
       <c r="F9" s="2" t="b">
         <f>C9&lt;=E9</f>
         <v>1</v>
@@ -671,11 +683,16 @@
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <f>4*E2+2*E3</f>
+        <v>20</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>20</v>
+      </c>
       <c r="F10" s="2" t="b">
         <f>C10&lt;=E10</f>
         <v>1</v>
@@ -685,11 +702,16 @@
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <f>E2</f>
+        <v>2.5</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
       <c r="F11" s="2" t="b">
         <f>C11&gt;=E11</f>
         <v>1</v>
@@ -699,11 +721,16 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <f>E3</f>
+        <v>5</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
       <c r="F12" s="2" t="b">
         <f>C12&gt;=E12</f>
         <v>1</v>
@@ -743,13 +770,17 @@
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>10.466805390419914</v>
+      </c>
     </row>
     <row r="3" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="D3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5">
+        <v>-100</v>
+      </c>
     </row>
     <row r="5" spans="2:6" ht="16" x14ac:dyDescent="0.15">
       <c r="C5" s="10" t="s">
@@ -765,7 +796,10 @@
       <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9">
+        <f>(E2^2)+E2*E3</f>
+        <v>-937.12652396106796</v>
+      </c>
     </row>
     <row r="8" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="C8" s="11" t="s">
@@ -778,25 +812,35 @@
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <f>(E2^3)+E2*E3</f>
+        <v>100.00001654916196</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>100</v>
+      </c>
       <c r="F9" s="2" t="b">
         <f>C9=E9</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <f>(E2^3)+E2*E3</f>
+        <v>100.00001654916196</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1">
+        <v>50</v>
+      </c>
       <c r="F10" s="2" t="b">
         <f>C10&gt;=E10</f>
         <v>1</v>
@@ -806,11 +850,16 @@
       <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>-100</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <f>E2</f>
+        <v>10.466805390419914</v>
+      </c>
       <c r="F11" s="2" t="b">
         <f>C11&lt;=E11</f>
         <v>1</v>
@@ -820,11 +869,16 @@
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <f>E2</f>
+        <v>10.466805390419914</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>100</v>
+      </c>
       <c r="F12" s="2" t="b">
         <f t="shared" ref="F12:F14" si="0">C12&lt;=E12</f>
         <v>1</v>
@@ -834,11 +888,16 @@
       <c r="B13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>-100</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <f>E3</f>
+        <v>-100</v>
+      </c>
       <c r="F13" s="2" t="b">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -848,11 +907,16 @@
       <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <f>E3</f>
+        <v>-100</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1">
+        <v>100</v>
+      </c>
       <c r="F14" s="2" t="b">
         <f t="shared" si="0"/>
         <v>1</v>

</xml_diff>